<commit_message>
token refresh in backend and frontend services
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE58C25-61DD-41C7-A847-E37983FF8206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264164C2-CD91-4C17-9E2F-4C395926974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$40</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t>Feature</t>
   </si>
@@ -271,6 +271,21 @@
   </si>
   <si>
     <t xml:space="preserve">Button hat nur Icon ohne Kreis (siehe WhatsApp Senden Button). </t>
+  </si>
+  <si>
+    <t>Voting API Call für userHasVoted ausbauen</t>
+  </si>
+  <si>
+    <t>Die Information, dass ein User bereits gevotet hat muss nicht von der API geladen werden</t>
+  </si>
+  <si>
+    <t>API Call für alle User die an einem Voting teilgenommen haben</t>
+  </si>
+  <si>
+    <t>voting closed view</t>
+  </si>
+  <si>
+    <t>Ein API Call der alle User mit allen Daten zu einem Voting zurück gibt</t>
   </si>
 </sst>
 </file>
@@ -317,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -329,10 +344,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -613,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +667,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -771,7 +782,7 @@
       <c r="B8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8"/>
       <c r="D8" t="s">
         <v>79</v>
       </c>
@@ -828,7 +839,7 @@
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12"/>
       <c r="E12" s="1" t="s">
         <v>20</v>
       </c>
@@ -903,216 +914,234 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>5</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="3" t="s">
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+        <v>55</v>
+      </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="3"/>
     </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I38" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I34">
-      <sortCondition ref="A1:A38"/>
+  <autoFilter ref="A1:I40" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
+      <sortCondition ref="A1:A40"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
A lot of refactoring & first implementation of profile view for users (WIP)
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIND\WIND\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264164C2-CD91-4C17-9E2F-4C395926974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5BDFD0-C6F4-40BD-AC79-09C15150D7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Feature</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>Ein API Call der alle User mit allen Daten zu einem Voting zurück gibt</t>
+  </si>
+  <si>
+    <t>Organisationen anpassen</t>
+  </si>
+  <si>
+    <t>Diskussion, Registrierung und ggf. Profile Edit View</t>
+  </si>
+  <si>
+    <t>Organisationen benötigen auf den Screens Diskussion und Registrierung jeweils Bilder (ggf. auch Profile Edit View). Beim Registrieren sowie abrufen der Daten muss ebenfalls die Reihenfolge gesetzt / geladen werden können. Die drei wichtigstens sieht man dann in den Diskussionen. Der Rest auf dem Profil (maximale Anzahl sinnvoll -&gt; z. B. max 5)</t>
   </si>
 </sst>
 </file>
@@ -624,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,47 +784,47 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C8"/>
-      <c r="D8" t="s">
+      <c r="C9"/>
+      <c r="D9" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -823,13 +832,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -837,271 +846,268 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12"/>
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C13"/>
       <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D15" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>6</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="1" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1110,38 +1116,55 @@
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
-      <c r="B33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="B34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="3"/>
     </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I40" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I36">
-      <sortCondition ref="A1:A40"/>
+  <autoFilter ref="A1:I41" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
+      <sortCondition ref="A1:A41"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added basic word list filtering for discussion posts
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5BDFD0-C6F4-40BD-AC79-09C15150D7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD88559B-2AB2-414C-A931-21BB52BEB0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="3930" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -353,6 +359,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -635,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,24 +685,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -713,76 +723,72 @@
       <c r="H3"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8">

</xml_diff>

<commit_message>
Fixed appearance and colors
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD88559B-2AB2-414C-A931-21BB52BEB0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C1BD88-1241-4905-B39C-4A06F604D320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,24 +704,21 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -790,19 +787,21 @@
       </c>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">

</xml_diff>

<commit_message>
finished features, changed order
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C1BD88-1241-4905-B39C-4A06F604D320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF822A7-E33D-4CC3-9A0A-A650E3C83C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28755" yWindow="-3345" windowWidth="25875" windowHeight="20850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -315,18 +315,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -347,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -359,10 +353,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -646,7 +636,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,165 +675,165 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>1</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C9"/>
-      <c r="D9" t="s">
+      <c r="C10"/>
+      <c r="D10" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -851,13 +841,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -865,42 +855,42 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13"/>
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C14"/>
       <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>8</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -917,7 +907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -931,7 +921,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -942,7 +932,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -953,7 +943,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>83</v>
       </c>
@@ -964,7 +954,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>75</v>
       </c>
@@ -975,7 +965,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -989,21 +979,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>5</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -1017,154 +1007,102 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
+    </row>
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
+    </row>
+    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+    </row>
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
+    </row>
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
+    </row>
+    <row r="33" spans="2:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+    </row>
+    <row r="34" spans="2:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
+    </row>
+    <row r="35" spans="2:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I41" xr:uid="{00000000-0001-0000-0000-000000000000}">

</xml_diff>

<commit_message>
Added round button to discussion send button and removed haptic feedback on news
</commit_message>
<xml_diff>
--- a/Documents/Feature Liste.xlsx
+++ b/Documents/Feature Liste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WIND\WIND\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevelopmentWIND\WIND\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF822A7-E33D-4CC3-9A0A-A650E3C83C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A775A62-887D-4838-94FA-355593D8DD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28755" yWindow="-3345" windowWidth="25875" windowHeight="20850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,19 +793,21 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -836,19 +838,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -907,7 +911,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -921,98 +925,106 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>5</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>6</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
@@ -1023,7 +1035,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1045,7 +1057,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>52</v>
       </c>
@@ -1053,7 +1065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
@@ -1061,12 +1073,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
@@ -1106,7 +1118,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I41" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I37">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I35">
       <sortCondition ref="A1:A41"/>
     </sortState>
   </autoFilter>

</xml_diff>